<commit_message>
Beds and GPR Addition
</commit_message>
<xml_diff>
--- a/outputdata.xlsx
+++ b/outputdata.xlsx
@@ -2235,7 +2235,9 @@
       <c r="I53" t="n">
         <v>2557413</v>
       </c>
-      <c r="J53" t="inlineStr"/>
+      <c r="J53" t="n">
+        <v>294.1764705882353</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr"/>
@@ -2253,7 +2255,9 @@
       <c r="I54" t="n">
         <v>902870</v>
       </c>
-      <c r="J54" t="inlineStr"/>
+      <c r="J54" t="n">
+        <v>294.1764705882353</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
State by state violation resaved
</commit_message>
<xml_diff>
--- a/outputdata.xlsx
+++ b/outputdata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,47 +441,57 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Facility Total</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Monthly</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Annual</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Employee Average</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Staff Increase/Decrease</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Population 2023</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Total Deficiencies</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Fines</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Sum of Fines</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Facility Total</t>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Certified Beds by State</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Gross Patient Revenue</t>
         </is>
       </c>
     </row>
@@ -492,31 +502,37 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>225</v>
+      </c>
+      <c r="C2" t="n">
         <v>8012</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>96144</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>19238.77777777778</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.09617449009466185</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>5056005</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>535</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>54</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>851118</v>
       </c>
-      <c r="J2" t="n">
-        <v>225</v>
+      <c r="K2" t="n">
+        <v>26573</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2122719</v>
       </c>
     </row>
     <row r="3">
@@ -526,31 +542,37 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" t="n">
         <v>37814</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>453768</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>581.7777777777778</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0.2512</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>731721</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>2258</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>244</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>2078926</v>
       </c>
-      <c r="J3" t="n">
-        <v>20</v>
+      <c r="K3" t="n">
+        <v>720</v>
+      </c>
+      <c r="L3" t="n">
+        <v>165283</v>
       </c>
     </row>
     <row r="4">
@@ -560,31 +582,37 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>142</v>
+      </c>
+      <c r="C4" t="n">
         <v>7848</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>94176</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>14836.11111111111</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.1309341500765697</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>7408017</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>6039</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>346</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>3670366</v>
       </c>
-      <c r="J4" t="n">
-        <v>142</v>
+      <c r="K4" t="n">
+        <v>15828</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1934486</v>
       </c>
     </row>
     <row r="5">
@@ -594,31 +622,37 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>218</v>
+      </c>
+      <c r="C5" t="n">
         <v>7300</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>87600</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>10633.44444444445</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.1041940285439103</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>3042231</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>3066</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>191</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>1130158</v>
       </c>
-      <c r="J5" t="n">
-        <v>218</v>
+      <c r="K5" t="n">
+        <v>24928</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1740574</v>
       </c>
     </row>
     <row r="6">
@@ -628,31 +662,37 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>1170</v>
+      </c>
+      <c r="C6" t="n">
         <v>11753</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>141036</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>91049.22222222222</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>0.1425659619796788</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>38959247</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>52680</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>2765</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>23922459</v>
       </c>
-      <c r="J6" t="n">
-        <v>1170</v>
+      <c r="K6" t="n">
+        <v>113562</v>
+      </c>
+      <c r="L6" t="n">
+        <v>15833208</v>
       </c>
     </row>
     <row r="7">
@@ -662,31 +702,37 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>218</v>
+      </c>
+      <c r="C7" t="n">
         <v>10281</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>123372</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>14047.55555555555</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0.08539621075923109</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>5855078</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>5030</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>806</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>10149862</v>
       </c>
-      <c r="J7" t="n">
-        <v>218</v>
+      <c r="K7" t="n">
+        <v>20179</v>
+      </c>
+      <c r="L7" t="n">
+        <v>2201353</v>
       </c>
     </row>
     <row r="8">
@@ -696,31 +742,37 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>203</v>
+      </c>
+      <c r="C8" t="n">
         <v>16516</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>198192</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>18894.22222222222</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>0.1014821536600121</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>3609924</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>5724</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>386</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>6550825</v>
       </c>
-      <c r="J8" t="n">
-        <v>203</v>
+      <c r="K8" t="n">
+        <v>26881</v>
+      </c>
+      <c r="L8" t="n">
+        <v>3763507</v>
       </c>
     </row>
     <row r="9">
@@ -730,31 +782,37 @@
         </is>
       </c>
       <c r="B9" t="n">
+        <v>44</v>
+      </c>
+      <c r="C9" t="n">
         <v>14728</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>176736</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>1976.222222222222</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>0.03778337531486146</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>1012615</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>896</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>55</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>2412409</v>
       </c>
-      <c r="J9" t="n">
-        <v>44</v>
+      <c r="K9" t="n">
+        <v>4384</v>
+      </c>
+      <c r="L9" t="n">
+        <v>699492</v>
       </c>
     </row>
     <row r="10">
@@ -764,31 +822,37 @@
         </is>
       </c>
       <c r="B10" t="n">
+        <v>17</v>
+      </c>
+      <c r="C10" t="n">
         <v>12593</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>151116</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>3475.555555555556</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>0.1039387308533917</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>22040323</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>1628</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>71</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>1616516</v>
       </c>
-      <c r="J10" t="n">
-        <v>17</v>
+      <c r="K10" t="n">
+        <v>2674</v>
+      </c>
+      <c r="L10" t="n">
+        <v>424978</v>
       </c>
     </row>
     <row r="11">
@@ -798,31 +862,37 @@
         </is>
       </c>
       <c r="B11" t="n">
+        <v>697</v>
+      </c>
+      <c r="C11" t="n">
         <v>10384</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>124608</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>66926.88888888889</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>0.1100849700515392</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>10852484</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>12515</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>1542</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>25616117</v>
       </c>
-      <c r="J11" t="n">
-        <v>697</v>
+      <c r="K11" t="n">
+        <v>88185</v>
+      </c>
+      <c r="L11" t="n">
+        <v>10721617</v>
       </c>
     </row>
     <row r="12">
@@ -832,31 +902,37 @@
         </is>
       </c>
       <c r="B12" t="n">
+        <v>357</v>
+      </c>
+      <c r="C12" t="n">
         <v>8413</v>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>100956</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>27631</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>0.08792816082179666</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>1433336</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>4594</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>738</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>8764323</v>
       </c>
-      <c r="J12" t="n">
-        <v>357</v>
+      <c r="K12" t="n">
+        <v>39695</v>
+      </c>
+      <c r="L12" t="n">
+        <v>4334554</v>
       </c>
     </row>
     <row r="13">
@@ -866,31 +942,37 @@
         </is>
       </c>
       <c r="B13" t="n">
+        <v>43</v>
+      </c>
+      <c r="C13" t="n">
         <v>15002</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>180024</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>3159.666666666667</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>-0.01564495530012771</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>1981332</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>46</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>3</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>7150</v>
       </c>
-      <c r="J13" t="n">
-        <v>43</v>
+      <c r="K13" t="n">
+        <v>4296</v>
+      </c>
+      <c r="L13" t="n">
+        <v>604409</v>
       </c>
     </row>
     <row r="14">
@@ -900,31 +982,37 @@
         </is>
       </c>
       <c r="B14" t="n">
+        <v>80</v>
+      </c>
+      <c r="C14" t="n">
         <v>10220</v>
       </c>
-      <c r="C14" t="n">
+      <c r="D14" t="n">
         <v>122640</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>19686</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>0.03873150532747564</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>12518144</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>1365</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>113</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>2178596</v>
       </c>
-      <c r="J14" t="n">
-        <v>80</v>
+      <c r="K14" t="n">
+        <v>6486</v>
+      </c>
+      <c r="L14" t="n">
+        <v>632175</v>
       </c>
     </row>
     <row r="15">
@@ -934,31 +1022,37 @@
         </is>
       </c>
       <c r="B15" t="n">
+        <v>694</v>
+      </c>
+      <c r="C15" t="n">
         <v>7519</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>90228</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>3657.888888888889</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>0.09102434077079108</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>6831167</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>8519</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>946</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>13234798</v>
       </c>
-      <c r="J15" t="n">
-        <v>694</v>
+      <c r="K15" t="n">
+        <v>81367</v>
+      </c>
+      <c r="L15" t="n">
+        <v>7559970</v>
       </c>
     </row>
     <row r="16">
@@ -968,31 +1062,37 @@
         </is>
       </c>
       <c r="B16" t="n">
+        <v>521</v>
+      </c>
+      <c r="C16" t="n">
         <v>8724</v>
       </c>
-      <c r="C16" t="n">
+      <c r="D16" t="n">
         <v>104688</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>56573.55555555555</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>0.1296633227061043</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>3196911</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>2189</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>184</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>2486095</v>
       </c>
-      <c r="J16" t="n">
-        <v>521</v>
+      <c r="K16" t="n">
+        <v>52181</v>
+      </c>
+      <c r="L16" t="n">
+        <v>5330743</v>
       </c>
     </row>
     <row r="17">
@@ -1002,31 +1102,37 @@
         </is>
       </c>
       <c r="B17" t="n">
+        <v>412</v>
+      </c>
+      <c r="C17" t="n">
         <v>8249</v>
       </c>
-      <c r="C17" t="n">
+      <c r="D17" t="n">
         <v>98988</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>33906.77777777778</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>0.08988636039987469</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>2928419</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>24341</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>2389</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>69986533</v>
       </c>
-      <c r="J17" t="n">
-        <v>412</v>
+      <c r="K17" t="n">
+        <v>28558</v>
+      </c>
+      <c r="L17" t="n">
+        <v>2507578</v>
       </c>
     </row>
     <row r="18">
@@ -1036,31 +1142,37 @@
         </is>
       </c>
       <c r="B18" t="n">
+        <v>313</v>
+      </c>
+      <c r="C18" t="n">
         <v>7556</v>
       </c>
-      <c r="C18" t="n">
+      <c r="D18" t="n">
         <v>90672</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>14469.88888888889</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>0.05267102752793677</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>4519315</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>14688</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>1325</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>17961843</v>
       </c>
-      <c r="J18" t="n">
-        <v>313</v>
+      <c r="K18" t="n">
+        <v>19884</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1874096</v>
       </c>
     </row>
     <row r="19">
@@ -1070,31 +1182,37 @@
         </is>
       </c>
       <c r="B19" t="n">
+        <v>276</v>
+      </c>
+      <c r="C19" t="n">
         <v>8614</v>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>103368</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>20069.66666666667</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>0.06845558711193811</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>4576882</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>7024</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>815</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>8183388</v>
       </c>
-      <c r="J19" t="n">
-        <v>276</v>
+      <c r="K19" t="n">
+        <v>27146</v>
+      </c>
+      <c r="L19" t="n">
+        <v>2647675</v>
       </c>
     </row>
     <row r="20">
@@ -1104,31 +1222,37 @@
         </is>
       </c>
       <c r="B20" t="n">
+        <v>269</v>
+      </c>
+      <c r="C20" t="n">
         <v>6911</v>
       </c>
-      <c r="C20" t="n">
+      <c r="D20" t="n">
         <v>82932</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>21796.55555555555</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>0.07328751939702949</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>1381441</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>3928</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>396</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>8871531</v>
       </c>
-      <c r="J20" t="n">
-        <v>269</v>
+      <c r="K20" t="n">
+        <v>34044</v>
+      </c>
+      <c r="L20" t="n">
+        <v>2284489</v>
       </c>
     </row>
     <row r="21">
@@ -1138,31 +1262,37 @@
         </is>
       </c>
       <c r="B21" t="n">
+        <v>87</v>
+      </c>
+      <c r="C21" t="n">
         <v>12593</v>
       </c>
-      <c r="C21" t="n">
+      <c r="D21" t="n">
         <v>151116</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>31527.88888888889</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>0.0834714294482293</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>6157731</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>4575</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>562</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>6286290</v>
       </c>
-      <c r="J21" t="n">
-        <v>87</v>
+      <c r="K21" t="n">
+        <v>6253</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1167318</v>
       </c>
     </row>
     <row r="22">
@@ -1172,31 +1302,37 @@
         </is>
       </c>
       <c r="B22" t="n">
+        <v>225</v>
+      </c>
+      <c r="C22" t="n">
         <v>12410</v>
       </c>
-      <c r="C22" t="n">
+      <c r="D22" t="n">
         <v>148920</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>21272.88888888889</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>0.1201191852708352</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>6962372</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>11350</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>958</v>
       </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
         <v>20331026</v>
       </c>
-      <c r="J22" t="n">
-        <v>225</v>
+      <c r="K22" t="n">
+        <v>28158</v>
+      </c>
+      <c r="L22" t="n">
+        <v>3766289</v>
       </c>
     </row>
     <row r="23">
@@ -1206,31 +1342,37 @@
         </is>
       </c>
       <c r="B23" t="n">
+        <v>353</v>
+      </c>
+      <c r="C23" t="n">
         <v>15148</v>
       </c>
-      <c r="C23" t="n">
+      <c r="D23" t="n">
         <v>181776</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>4887.111111111111</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>0.04457973291437549</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>10032720</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>9461</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>348</v>
       </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
         <v>4825443</v>
       </c>
-      <c r="J23" t="n">
-        <v>353</v>
+      <c r="K23" t="n">
+        <v>46029</v>
+      </c>
+      <c r="L23" t="n">
+        <v>5932813</v>
       </c>
     </row>
     <row r="24">
@@ -1240,31 +1382,37 @@
         </is>
       </c>
       <c r="B24" t="n">
+        <v>430</v>
+      </c>
+      <c r="C24" t="n">
         <v>10914</v>
       </c>
-      <c r="C24" t="n">
+      <c r="D24" t="n">
         <v>130968</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>31645.77777777778</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>0.09097992208570573</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>5702253</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>1610</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>89</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
         <v>732234</v>
       </c>
-      <c r="J24" t="n">
-        <v>430</v>
+      <c r="K24" t="n">
+        <v>47102</v>
+      </c>
+      <c r="L24" t="n">
+        <v>5868040</v>
       </c>
     </row>
     <row r="25">
@@ -1274,31 +1422,37 @@
         </is>
       </c>
       <c r="B25" t="n">
+        <v>353</v>
+      </c>
+      <c r="C25" t="n">
         <v>13921</v>
       </c>
-      <c r="C25" t="n">
+      <c r="D25" t="n">
         <v>167052</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>19658.44444444445</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>0.01714973422926487</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>2940820</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>16644</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>1189</v>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
         <v>35999121</v>
       </c>
-      <c r="J25" t="n">
-        <v>353</v>
+      <c r="K25" t="n">
+        <v>26576</v>
+      </c>
+      <c r="L25" t="n">
+        <v>2765837</v>
       </c>
     </row>
     <row r="26">
@@ -1308,31 +1462,37 @@
         </is>
       </c>
       <c r="B26" t="n">
+        <v>202</v>
+      </c>
+      <c r="C26" t="n">
         <v>8541</v>
       </c>
-      <c r="C26" t="n">
+      <c r="D26" t="n">
         <v>102492</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>31743.22222222222</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>0.1296163499462173</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>6180523</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>8265</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>826</v>
       </c>
-      <c r="I26" t="n">
+      <c r="J26" t="n">
         <v>14075722</v>
       </c>
-      <c r="J26" t="n">
-        <v>202</v>
+      <c r="K26" t="n">
+        <v>16464</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1441731</v>
       </c>
     </row>
     <row r="27">
@@ -1342,31 +1502,37 @@
         </is>
       </c>
       <c r="B27" t="n">
+        <v>510</v>
+      </c>
+      <c r="C27" t="n">
         <v>6315</v>
       </c>
-      <c r="C27" t="n">
+      <c r="D27" t="n">
         <v>75780</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>13617</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>0.07864771200226324</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>1125473</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>15833</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>1778</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>21549250</v>
       </c>
-      <c r="J27" t="n">
-        <v>510</v>
+      <c r="K27" t="n">
+        <v>54977</v>
+      </c>
+      <c r="L27" t="n">
+        <v>3829977</v>
       </c>
     </row>
     <row r="28">
@@ -1376,31 +1542,37 @@
         </is>
       </c>
       <c r="B28" t="n">
+        <v>62</v>
+      </c>
+      <c r="C28" t="n">
         <v>9089</v>
       </c>
-      <c r="C28" t="n">
+      <c r="D28" t="n">
         <v>109068</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>3158.666666666667</v>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>0.006620428751576293</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>1966441</v>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>2634</v>
       </c>
-      <c r="H28" t="n">
+      <c r="I28" t="n">
         <v>227</v>
       </c>
-      <c r="I28" t="n">
+      <c r="J28" t="n">
         <v>4617342</v>
       </c>
-      <c r="J28" t="n">
-        <v>62</v>
+      <c r="K28" t="n">
+        <v>5644</v>
+      </c>
+      <c r="L28" t="n">
+        <v>315947</v>
       </c>
     </row>
     <row r="29">
@@ -1410,31 +1582,37 @@
         </is>
       </c>
       <c r="B29" t="n">
+        <v>185</v>
+      </c>
+      <c r="C29" t="n">
         <v>8979</v>
       </c>
-      <c r="C29" t="n">
+      <c r="D29" t="n">
         <v>107748</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>31356</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>0.129995126705653</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>3201212</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>1389</v>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>293</v>
       </c>
-      <c r="I29" t="n">
+      <c r="J29" t="n">
         <v>4562038</v>
       </c>
-      <c r="J29" t="n">
-        <v>185</v>
+      <c r="K29" t="n">
+        <v>15256</v>
+      </c>
+      <c r="L29" t="n">
+        <v>1305705</v>
       </c>
     </row>
     <row r="30">
@@ -1444,31 +1622,37 @@
         </is>
       </c>
       <c r="B30" t="n">
+        <v>67</v>
+      </c>
+      <c r="C30" t="n">
         <v>11060</v>
       </c>
-      <c r="C30" t="n">
+      <c r="D30" t="n">
         <v>132720</v>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
         <v>4445.666666666667</v>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>0.04958492259367287</v>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>1405243</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>8349</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>825</v>
       </c>
-      <c r="I30" t="n">
+      <c r="J30" t="n">
         <v>22107564</v>
       </c>
-      <c r="J30" t="n">
-        <v>67</v>
+      <c r="K30" t="n">
+        <v>6860</v>
+      </c>
+      <c r="L30" t="n">
+        <v>891435</v>
       </c>
     </row>
     <row r="31">
@@ -1478,31 +1662,37 @@
         </is>
       </c>
       <c r="B31" t="n">
+        <v>73</v>
+      </c>
+      <c r="C31" t="n">
         <v>13140</v>
       </c>
-      <c r="C31" t="n">
+      <c r="D31" t="n">
         <v>157680</v>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
         <v>9359.222222222223</v>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>0.03264221158958001</v>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>9242109</v>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>1256</v>
       </c>
-      <c r="H31" t="n">
+      <c r="I31" t="n">
         <v>104</v>
       </c>
-      <c r="I31" t="n">
+      <c r="J31" t="n">
         <v>1146282</v>
       </c>
-      <c r="J31" t="n">
-        <v>73</v>
+      <c r="K31" t="n">
+        <v>6937</v>
+      </c>
+      <c r="L31" t="n">
+        <v>904564</v>
       </c>
     </row>
     <row r="32">
@@ -1512,31 +1702,37 @@
         </is>
       </c>
       <c r="B32" t="n">
+        <v>348</v>
+      </c>
+      <c r="C32" t="n">
         <v>13504</v>
       </c>
-      <c r="C32" t="n">
+      <c r="D32" t="n">
         <v>162048</v>
       </c>
-      <c r="D32" t="n">
+      <c r="E32" t="n">
         <v>5484.777777777777</v>
       </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
         <v>0.06004945249028612</v>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>2113550</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>3744</v>
       </c>
-      <c r="H32" t="n">
+      <c r="I32" t="n">
         <v>369</v>
       </c>
-      <c r="I32" t="n">
+      <c r="J32" t="n">
         <v>3628833</v>
       </c>
-      <c r="J32" t="n">
-        <v>348</v>
+      <c r="K32" t="n">
+        <v>54015</v>
+      </c>
+      <c r="L32" t="n">
+        <v>6372948</v>
       </c>
     </row>
     <row r="33">
@@ -1546,31 +1742,37 @@
         </is>
       </c>
       <c r="B33" t="n">
+        <v>68</v>
+      </c>
+      <c r="C33" t="n">
         <v>9125</v>
       </c>
-      <c r="C33" t="n">
+      <c r="D33" t="n">
         <v>109500</v>
       </c>
-      <c r="D33" t="n">
+      <c r="E33" t="n">
         <v>37192.11111111111</v>
       </c>
-      <c r="E33" t="n">
+      <c r="F33" t="n">
         <v>0.1084282344586197</v>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>19415392</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>1002</v>
       </c>
-      <c r="H33" t="n">
+      <c r="I33" t="n">
         <v>95</v>
       </c>
-      <c r="I33" t="n">
+      <c r="J33" t="n">
         <v>1049582</v>
       </c>
-      <c r="J33" t="n">
-        <v>68</v>
+      <c r="K33" t="n">
+        <v>7145</v>
+      </c>
+      <c r="L33" t="n">
+        <v>705338</v>
       </c>
     </row>
     <row r="34">
@@ -1580,31 +1782,37 @@
         </is>
       </c>
       <c r="B34" t="n">
+        <v>606</v>
+      </c>
+      <c r="C34" t="n">
         <v>15330</v>
       </c>
-      <c r="C34" t="n">
+      <c r="D34" t="n">
         <v>183960</v>
       </c>
-      <c r="D34" t="n">
+      <c r="E34" t="n">
         <v>4855.333333333333</v>
       </c>
-      <c r="E34" t="n">
+      <c r="F34" t="n">
         <v>0.1169085916045508</v>
       </c>
-      <c r="F34" t="n">
+      <c r="G34" t="n">
         <v>10678831</v>
       </c>
-      <c r="G34" t="n">
+      <c r="H34" t="n">
         <v>5182</v>
       </c>
-      <c r="H34" t="n">
+      <c r="I34" t="n">
         <v>803</v>
       </c>
-      <c r="I34" t="n">
+      <c r="J34" t="n">
         <v>12082855</v>
       </c>
-      <c r="J34" t="n">
-        <v>606</v>
+      <c r="K34" t="n">
+        <v>113414</v>
+      </c>
+      <c r="L34" t="n">
+        <v>16677396</v>
       </c>
     </row>
     <row r="35">
@@ -1614,31 +1822,37 @@
         </is>
       </c>
       <c r="B35" t="n">
+        <v>420</v>
+      </c>
+      <c r="C35" t="n">
         <v>8979</v>
       </c>
-      <c r="C35" t="n">
+      <c r="D35" t="n">
         <v>107748</v>
       </c>
-      <c r="D35" t="n">
+      <c r="E35" t="n">
         <v>5124.555555555556</v>
       </c>
-      <c r="E35" t="n">
+      <c r="F35" t="n">
         <v>0.1337325349301397</v>
       </c>
-      <c r="F35" t="n">
+      <c r="G35" t="n">
         <v>770221</v>
       </c>
-      <c r="G35" t="n">
+      <c r="H35" t="n">
         <v>2864</v>
       </c>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
         <v>244</v>
       </c>
-      <c r="I35" t="n">
+      <c r="J35" t="n">
         <v>4624593</v>
       </c>
-      <c r="J35" t="n">
-        <v>420</v>
+      <c r="K35" t="n">
+        <v>44738</v>
+      </c>
+      <c r="L35" t="n">
+        <v>4838162</v>
       </c>
     </row>
     <row r="36">
@@ -1648,31 +1862,37 @@
         </is>
       </c>
       <c r="B36" t="n">
+        <v>77</v>
+      </c>
+      <c r="C36" t="n">
         <v>14374</v>
       </c>
-      <c r="C36" t="n">
+      <c r="D36" t="n">
         <v>172488</v>
       </c>
-      <c r="D36" t="n">
+      <c r="E36" t="n">
         <v>92205.55555555556</v>
       </c>
-      <c r="E36" t="n">
+      <c r="F36" t="n">
         <v>0.09671179883945841</v>
       </c>
-      <c r="F36" t="n">
+      <c r="G36" t="n">
         <v>11767059</v>
       </c>
-      <c r="G36" t="n">
+      <c r="H36" t="n">
         <v>2815</v>
       </c>
-      <c r="H36" t="n">
+      <c r="I36" t="n">
         <v>263</v>
       </c>
-      <c r="I36" t="n">
+      <c r="J36" t="n">
         <v>1479126</v>
       </c>
-      <c r="J36" t="n">
-        <v>77</v>
+      <c r="K36" t="n">
+        <v>5109</v>
+      </c>
+      <c r="L36" t="n">
+        <v>527149</v>
       </c>
     </row>
     <row r="37">
@@ -1682,31 +1902,37 @@
         </is>
       </c>
       <c r="B37" t="n">
+        <v>946</v>
+      </c>
+      <c r="C37" t="n">
         <v>8760</v>
       </c>
-      <c r="C37" t="n">
+      <c r="D37" t="n">
         <v>105120</v>
       </c>
-      <c r="D37" t="n">
+      <c r="E37" t="n">
         <v>62399.11111111111</v>
       </c>
-      <c r="E37" t="n">
+      <c r="F37" t="n">
         <v>0.09668933263591889</v>
       </c>
-      <c r="F37" t="n">
+      <c r="G37" t="n">
         <v>4018931</v>
       </c>
-      <c r="G37" t="n">
+      <c r="H37" t="n">
         <v>9599</v>
       </c>
-      <c r="H37" t="n">
+      <c r="I37" t="n">
         <v>911</v>
       </c>
-      <c r="I37" t="n">
+      <c r="J37" t="n">
         <v>7053562</v>
       </c>
-      <c r="J37" t="n">
-        <v>946</v>
+      <c r="K37" t="n">
+        <v>91570</v>
+      </c>
+      <c r="L37" t="n">
+        <v>9053725</v>
       </c>
     </row>
     <row r="38">
@@ -1716,31 +1942,37 @@
         </is>
       </c>
       <c r="B38" t="n">
+        <v>292</v>
+      </c>
+      <c r="C38" t="n">
         <v>6570</v>
       </c>
-      <c r="C38" t="n">
+      <c r="D38" t="n">
         <v>78840</v>
       </c>
-      <c r="D38" t="n">
+      <c r="E38" t="n">
         <v>15212.22222222222</v>
       </c>
-      <c r="E38" t="n">
+      <c r="F38" t="n">
         <v>0.09074226412706449</v>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>4259743</v>
       </c>
-      <c r="G38" t="n">
+      <c r="H38" t="n">
         <v>27993</v>
       </c>
-      <c r="H38" t="n">
+      <c r="I38" t="n">
         <v>2245</v>
       </c>
-      <c r="I38" t="n">
+      <c r="J38" t="n">
         <v>35090149</v>
       </c>
-      <c r="J38" t="n">
-        <v>292</v>
+      <c r="K38" t="n">
+        <v>29677</v>
+      </c>
+      <c r="L38" t="n">
+        <v>1726879</v>
       </c>
     </row>
     <row r="39">
@@ -1750,31 +1982,37 @@
         </is>
       </c>
       <c r="B39" t="n">
+        <v>129</v>
+      </c>
+      <c r="C39" t="n">
         <v>12410</v>
       </c>
-      <c r="C39" t="n">
+      <c r="D39" t="n">
         <v>148920</v>
       </c>
-      <c r="D39" t="n">
+      <c r="E39" t="n">
         <v>6165.111111111111</v>
       </c>
-      <c r="E39" t="n">
+      <c r="F39" t="n">
         <v>-0.02856220751976763</v>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
         <v>12916089</v>
       </c>
-      <c r="G39" t="n">
+      <c r="H39" t="n">
         <v>7080</v>
       </c>
-      <c r="H39" t="n">
+      <c r="I39" t="n">
         <v>953</v>
       </c>
-      <c r="I39" t="n">
+      <c r="J39" t="n">
         <v>7787192</v>
       </c>
-      <c r="J39" t="n">
-        <v>129</v>
+      <c r="K39" t="n">
+        <v>10020</v>
+      </c>
+      <c r="L39" t="n">
+        <v>1248069</v>
       </c>
     </row>
     <row r="40">
@@ -1784,31 +2022,37 @@
         </is>
       </c>
       <c r="B40" t="n">
+        <v>672</v>
+      </c>
+      <c r="C40" t="n">
         <v>12484</v>
       </c>
-      <c r="C40" t="n">
+      <c r="D40" t="n">
         <v>149808</v>
       </c>
-      <c r="D40" t="n">
+      <c r="E40" t="n">
         <v>63692.77777777778</v>
       </c>
-      <c r="E40" t="n">
+      <c r="F40" t="n">
         <v>0.07261703970460866</v>
       </c>
-      <c r="F40" t="n">
+      <c r="G40" t="n">
         <v>1094843</v>
       </c>
-      <c r="G40" t="n">
+      <c r="H40" t="n">
         <v>4557</v>
       </c>
-      <c r="H40" t="n">
+      <c r="I40" t="n">
         <v>313</v>
       </c>
-      <c r="I40" t="n">
+      <c r="J40" t="n">
         <v>5199588</v>
       </c>
-      <c r="J40" t="n">
-        <v>672</v>
+      <c r="K40" t="n">
+        <v>86150</v>
+      </c>
+      <c r="L40" t="n">
+        <v>10964321</v>
       </c>
     </row>
     <row r="41">
@@ -1818,31 +2062,37 @@
         </is>
       </c>
       <c r="B41" t="n">
+        <v>75</v>
+      </c>
+      <c r="C41" t="n">
         <v>11315</v>
       </c>
-      <c r="C41" t="n">
+      <c r="D41" t="n">
         <v>135780</v>
       </c>
-      <c r="D41" t="n">
+      <c r="E41" t="n">
         <v>6467.333333333333</v>
       </c>
-      <c r="E41" t="n">
+      <c r="F41" t="n">
         <v>0.1341374800174393</v>
       </c>
-      <c r="F41" t="n">
+      <c r="G41" t="n">
         <v>5259222</v>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="n">
         <v>17419</v>
       </c>
-      <c r="H41" t="n">
+      <c r="I41" t="n">
         <v>1317</v>
       </c>
-      <c r="I41" t="n">
+      <c r="J41" t="n">
         <v>21494990</v>
       </c>
-      <c r="J41" t="n">
-        <v>75</v>
+      <c r="K41" t="n">
+        <v>8775</v>
+      </c>
+      <c r="L41" t="n">
+        <v>945672</v>
       </c>
     </row>
     <row r="42">
@@ -1852,31 +2102,37 @@
         </is>
       </c>
       <c r="B42" t="n">
+        <v>188</v>
+      </c>
+      <c r="C42" t="n">
         <v>8742</v>
       </c>
-      <c r="C42" t="n">
+      <c r="D42" t="n">
         <v>104904</v>
       </c>
-      <c r="D42" t="n">
+      <c r="E42" t="n">
         <v>15117.11111111111</v>
       </c>
-      <c r="E42" t="n">
+      <c r="F42" t="n">
         <v>0.09797361277697116</v>
       </c>
-      <c r="F42" t="n">
+      <c r="G42" t="n">
         <v>905404</v>
       </c>
-      <c r="G42" t="n">
+      <c r="H42" t="n">
         <v>112</v>
       </c>
-      <c r="H42" t="n">
+      <c r="I42" t="n">
         <v>47</v>
       </c>
-      <c r="I42" t="n">
+      <c r="J42" t="n">
         <v>352025</v>
       </c>
-      <c r="J42" t="n">
-        <v>188</v>
+      <c r="K42" t="n">
+        <v>19805</v>
+      </c>
+      <c r="L42" t="n">
+        <v>2258091</v>
       </c>
     </row>
     <row r="43">
@@ -1886,31 +2142,37 @@
         </is>
       </c>
       <c r="B43" t="n">
+        <v>98</v>
+      </c>
+      <c r="C43" t="n">
         <v>8541</v>
       </c>
-      <c r="C43" t="n">
+      <c r="D43" t="n">
         <v>102492</v>
       </c>
-      <c r="D43" t="n">
+      <c r="E43" t="n">
         <v>7072.333333333333</v>
       </c>
-      <c r="E43" t="n">
+      <c r="F43" t="n">
         <v>0.05562526139690506</v>
       </c>
-      <c r="F43" t="n">
+      <c r="G43" t="n">
         <v>7059618</v>
       </c>
-      <c r="G43" t="n">
+      <c r="H43" t="n">
         <v>1866</v>
       </c>
-      <c r="H43" t="n">
+      <c r="I43" t="n">
         <v>230</v>
       </c>
-      <c r="I43" t="n">
+      <c r="J43" t="n">
         <v>4727888</v>
       </c>
-      <c r="J43" t="n">
-        <v>98</v>
+      <c r="K43" t="n">
+        <v>5655</v>
+      </c>
+      <c r="L43" t="n">
+        <v>519646</v>
       </c>
     </row>
     <row r="44">
@@ -1920,31 +2182,37 @@
         </is>
       </c>
       <c r="B44" t="n">
+        <v>312</v>
+      </c>
+      <c r="C44" t="n">
         <v>8578</v>
       </c>
-      <c r="C44" t="n">
+      <c r="D44" t="n">
         <v>102936</v>
       </c>
-      <c r="D44" t="n">
+      <c r="E44" t="n">
         <v>19224.55555555555</v>
       </c>
-      <c r="E44" t="n">
+      <c r="F44" t="n">
         <v>0.08106219426974144</v>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>29947238</v>
       </c>
-      <c r="G44" t="n">
+      <c r="H44" t="n">
         <v>2850</v>
       </c>
-      <c r="H44" t="n">
+      <c r="I44" t="n">
         <v>352</v>
       </c>
-      <c r="I44" t="n">
+      <c r="J44" t="n">
         <v>4721542</v>
       </c>
-      <c r="J44" t="n">
-        <v>312</v>
+      <c r="K44" t="n">
+        <v>37034</v>
+      </c>
+      <c r="L44" t="n">
+        <v>3269653</v>
       </c>
     </row>
     <row r="45">
@@ -1954,31 +2222,37 @@
         </is>
       </c>
       <c r="B45" t="n">
+        <v>1195</v>
+      </c>
+      <c r="C45" t="n">
         <v>6150</v>
       </c>
-      <c r="C45" t="n">
+      <c r="D45" t="n">
         <v>73800</v>
       </c>
-      <c r="D45" t="n">
+      <c r="E45" t="n">
         <v>66427.88888888889</v>
       </c>
-      <c r="E45" t="n">
+      <c r="F45" t="n">
         <v>0.1077258018463881</v>
       </c>
-      <c r="F45" t="n">
+      <c r="G45" t="n">
         <v>3426431</v>
       </c>
-      <c r="G45" t="n">
+      <c r="H45" t="n">
         <v>1281</v>
       </c>
-      <c r="H45" t="n">
+      <c r="I45" t="n">
         <v>163</v>
       </c>
-      <c r="I45" t="n">
+      <c r="J45" t="n">
         <v>2013213</v>
       </c>
-      <c r="J45" t="n">
-        <v>1195</v>
+      <c r="K45" t="n">
+        <v>148392</v>
+      </c>
+      <c r="L45" t="n">
+        <v>9083651</v>
       </c>
     </row>
     <row r="46">
@@ -1988,31 +2262,37 @@
         </is>
       </c>
       <c r="B46" t="n">
+        <v>98</v>
+      </c>
+      <c r="C46" t="n">
         <v>8614</v>
       </c>
-      <c r="C46" t="n">
+      <c r="D46" t="n">
         <v>103368</v>
       </c>
-      <c r="D46" t="n">
+      <c r="E46" t="n">
         <v>22662.66666666667</v>
       </c>
-      <c r="E46" t="n">
+      <c r="F46" t="n">
         <v>0.1180791972764737</v>
       </c>
-      <c r="F46" t="n">
+      <c r="G46" t="n">
         <v>647378</v>
       </c>
-      <c r="G46" t="n">
+      <c r="H46" t="n">
         <v>4309</v>
       </c>
-      <c r="H46" t="n">
+      <c r="I46" t="n">
         <v>403</v>
       </c>
-      <c r="I46" t="n">
+      <c r="J46" t="n">
         <v>9324806</v>
       </c>
-      <c r="J46" t="n">
-        <v>98</v>
+      <c r="K46" t="n">
+        <v>8781</v>
+      </c>
+      <c r="L46" t="n">
+        <v>864580</v>
       </c>
     </row>
     <row r="47">
@@ -2022,31 +2302,37 @@
         </is>
       </c>
       <c r="B47" t="n">
+        <v>35</v>
+      </c>
+      <c r="C47" t="n">
         <v>12702</v>
       </c>
-      <c r="C47" t="n">
+      <c r="D47" t="n">
         <v>152424</v>
       </c>
-      <c r="D47" t="n">
+      <c r="E47" t="n">
         <v>20842.44444444445</v>
       </c>
-      <c r="E47" t="n">
+      <c r="F47" t="n">
         <v>0.1306595760395893</v>
       </c>
-      <c r="F47" t="n">
+      <c r="G47" t="n">
         <v>8662151</v>
       </c>
-      <c r="G47" t="n">
+      <c r="H47" t="n">
         <v>24058</v>
       </c>
-      <c r="H47" t="n">
+      <c r="I47" t="n">
         <v>3592</v>
       </c>
-      <c r="I47" t="n">
+      <c r="J47" t="n">
         <v>54442591</v>
       </c>
-      <c r="J47" t="n">
-        <v>35</v>
+      <c r="K47" t="n">
+        <v>2995</v>
+      </c>
+      <c r="L47" t="n">
+        <v>396837</v>
       </c>
     </row>
     <row r="48">
@@ -2056,31 +2342,37 @@
         </is>
       </c>
       <c r="B48" t="n">
+        <v>289</v>
+      </c>
+      <c r="C48" t="n">
         <v>9855</v>
       </c>
-      <c r="C48" t="n">
+      <c r="D48" t="n">
         <v>118260</v>
       </c>
-      <c r="D48" t="n">
+      <c r="E48" t="n">
         <v>7728.111111111111</v>
       </c>
-      <c r="E48" t="n">
+      <c r="F48" t="n">
         <v>0.08409189423493715</v>
       </c>
-      <c r="F48" t="n">
+      <c r="G48" t="n">
         <v>7765004</v>
       </c>
-      <c r="G48" t="n">
+      <c r="H48" t="n">
         <v>2646</v>
       </c>
-      <c r="H48" t="n">
+      <c r="I48" t="n">
         <v>275</v>
       </c>
-      <c r="I48" t="n">
+      <c r="J48" t="n">
         <v>3085350</v>
       </c>
-      <c r="J48" t="n">
-        <v>289</v>
+      <c r="K48" t="n">
+        <v>32149</v>
+      </c>
+      <c r="L48" t="n">
+        <v>4529315</v>
       </c>
     </row>
     <row r="49">
@@ -2090,31 +2382,37 @@
         </is>
       </c>
       <c r="B49" t="n">
+        <v>198</v>
+      </c>
+      <c r="C49" t="n">
         <v>11315</v>
       </c>
-      <c r="C49" t="n">
+      <c r="D49" t="n">
         <v>135780</v>
       </c>
-      <c r="D49" t="n">
+      <c r="E49" t="n">
         <v>9989.444444444445</v>
       </c>
-      <c r="E49" t="n">
+      <c r="F49" t="n">
         <v>0.09215413184772517</v>
       </c>
-      <c r="F49" t="n">
+      <c r="G49" t="n">
         <v>657185</v>
       </c>
-      <c r="G49" t="n">
+      <c r="H49" t="n">
         <v>10075</v>
       </c>
-      <c r="H49" t="n">
+      <c r="I49" t="n">
         <v>459</v>
       </c>
-      <c r="I49" t="n">
+      <c r="J49" t="n">
         <v>6496163</v>
       </c>
-      <c r="J49" t="n">
-        <v>198</v>
+      <c r="K49" t="n">
+        <v>20848</v>
+      </c>
+      <c r="L49" t="n">
+        <v>2510233</v>
       </c>
     </row>
     <row r="50">
@@ -2124,31 +2422,37 @@
         </is>
       </c>
       <c r="B50" t="n">
+        <v>123</v>
+      </c>
+      <c r="C50" t="n">
         <v>13943</v>
       </c>
-      <c r="C50" t="n">
+      <c r="D50" t="n">
         <v>167316</v>
       </c>
-      <c r="D50" t="n">
+      <c r="E50" t="n">
         <v>16504.55555555555</v>
       </c>
-      <c r="E50" t="n">
+      <c r="F50" t="n">
         <v>-0.03337396250507865</v>
       </c>
-      <c r="F50" t="n">
+      <c r="G50" t="n">
         <v>1773866</v>
       </c>
-      <c r="G50" t="n">
+      <c r="H50" t="n">
         <v>680</v>
       </c>
-      <c r="H50" t="n">
+      <c r="I50" t="n">
         <v>49</v>
       </c>
-      <c r="I50" t="n">
+      <c r="J50" t="n">
         <v>1287903</v>
       </c>
-      <c r="J50" t="n">
-        <v>123</v>
+      <c r="K50" t="n">
+        <v>10077</v>
+      </c>
+      <c r="L50" t="n">
+        <v>1259821</v>
       </c>
     </row>
     <row r="51">
@@ -2158,31 +2462,37 @@
         </is>
       </c>
       <c r="B51" t="n">
+        <v>332</v>
+      </c>
+      <c r="C51" t="n">
         <v>10826</v>
       </c>
-      <c r="C51" t="n">
+      <c r="D51" t="n">
         <v>129912</v>
       </c>
-      <c r="D51" t="n">
+      <c r="E51" t="n">
         <v>10618.11111111111</v>
       </c>
-      <c r="E51" t="n">
+      <c r="F51" t="n">
         <v>0.1058963797962281</v>
       </c>
-      <c r="F51" t="n">
+      <c r="G51" t="n">
         <v>5903573</v>
       </c>
-      <c r="G51" t="n">
+      <c r="H51" t="n">
         <v>10457</v>
       </c>
-      <c r="H51" t="n">
+      <c r="I51" t="n">
         <v>526</v>
       </c>
-      <c r="I51" t="n">
+      <c r="J51" t="n">
         <v>14011082</v>
       </c>
-      <c r="J51" t="n">
-        <v>332</v>
+      <c r="K51" t="n">
+        <v>29089</v>
+      </c>
+      <c r="L51" t="n">
+        <v>2755982</v>
       </c>
     </row>
     <row r="52">
@@ -2192,31 +2502,37 @@
         </is>
       </c>
       <c r="B52" t="n">
+        <v>36</v>
+      </c>
+      <c r="C52" t="n">
         <v>8395</v>
       </c>
-      <c r="C52" t="n">
+      <c r="D52" t="n">
         <v>100740</v>
       </c>
-      <c r="D52" t="n">
+      <c r="E52" t="n">
         <v>3555.555555555556</v>
       </c>
-      <c r="E52" t="n">
+      <c r="F52" t="n">
         <v>0.03368526897938662</v>
       </c>
-      <c r="F52" t="n">
+      <c r="G52" t="n">
         <v>581813</v>
       </c>
-      <c r="G52" t="n">
+      <c r="H52" t="n">
         <v>7738</v>
       </c>
-      <c r="H52" t="n">
+      <c r="I52" t="n">
         <v>778</v>
       </c>
-      <c r="I52" t="n">
+      <c r="J52" t="n">
         <v>19119175</v>
       </c>
-      <c r="J52" t="n">
-        <v>36</v>
+      <c r="K52" t="n">
+        <v>2589</v>
+      </c>
+      <c r="L52" t="n">
+        <v>235530</v>
       </c>
     </row>
     <row r="53">
@@ -2226,18 +2542,18 @@
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
-      <c r="G53" t="n">
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="n">
         <v>4327</v>
       </c>
-      <c r="H53" t="n">
+      <c r="I53" t="n">
         <v>154</v>
       </c>
-      <c r="I53" t="n">
+      <c r="J53" t="n">
         <v>2557413</v>
       </c>
-      <c r="J53" t="n">
-        <v>294.1764705882353</v>
-      </c>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr"/>
@@ -2246,18 +2562,18 @@
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
-      <c r="G54" t="n">
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="n">
         <v>693</v>
       </c>
-      <c r="H54" t="n">
+      <c r="I54" t="n">
         <v>102</v>
       </c>
-      <c r="I54" t="n">
+      <c r="J54" t="n">
         <v>902870</v>
       </c>
-      <c r="J54" t="n">
-        <v>294.1764705882353</v>
-      </c>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>